<commit_message>
lab4 FoDM & APiPL 2 rep
</commit_message>
<xml_diff>
--- a/3-2 labs.xlsx
+++ b/3-2 labs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSTU\3\3-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57033989-6C9E-4B41-8435-8DB584F65B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82024BB8-4830-410A-89CA-AE7CB0A8DC08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3CBCB977-0A19-4CE0-8F0F-0CE5EBE89482}"/>
   </bookViews>
@@ -130,7 +130,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -140,12 +140,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -240,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -284,16 +278,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -318,19 +309,19 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -653,7 +644,7 @@
   <dimension ref="A1:Y19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -738,8 +729,8 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="35"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="33"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
@@ -763,15 +754,15 @@
       </c>
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
-      <c r="Y2" s="20"/>
+      <c r="Y2" s="19"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="20"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
@@ -784,7 +775,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
-      <c r="Q3" s="30" t="s">
+      <c r="Q3" s="29" t="s">
         <v>1</v>
       </c>
       <c r="R3" s="8"/>
@@ -794,19 +785,19 @@
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="29" t="s">
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="28" t="s">
         <v>1</v>
       </c>
       <c r="O4" s="8"/>
@@ -819,8 +810,8 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="11"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -831,9 +822,9 @@
       <c r="K5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="23"/>
+      <c r="L5" s="22"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="24"/>
+      <c r="N5" s="23"/>
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
@@ -844,16 +835,16 @@
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="34">
+      <c r="B6" s="32">
         <v>4</v>
       </c>
-      <c r="C6" s="33"/>
+      <c r="C6" s="35"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
-      <c r="I6" s="26" t="s">
+      <c r="I6" s="25" t="s">
         <v>12</v>
       </c>
       <c r="J6" s="8"/>
@@ -868,13 +859,13 @@
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="21"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="9"/>
       <c r="D7" s="10"/>
       <c r="E7" s="9"/>
       <c r="F7" s="10"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="25" t="s">
+      <c r="H7" s="24" t="s">
         <v>1</v>
       </c>
       <c r="L7" s="8"/>
@@ -890,8 +881,8 @@
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="36"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
@@ -915,12 +906,12 @@
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="19"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="29" t="s">
         <v>12</v>
       </c>
       <c r="H9" s="8"/>

</xml_diff>

<commit_message>
lab5 FoDM, PM,AiPL 3 lab, ISaRIS lab 5
</commit_message>
<xml_diff>
--- a/3-2 labs.xlsx
+++ b/3-2 labs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSTU\3\3-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82024BB8-4830-410A-89CA-AE7CB0A8DC08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D0A1B9-86D1-438D-9643-299BC3F86C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3CBCB977-0A19-4CE0-8F0F-0CE5EBE89482}"/>
+    <workbookView xWindow="0" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{3CBCB977-0A19-4CE0-8F0F-0CE5EBE89482}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -163,7 +163,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.499984740745262"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -318,13 +318,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -644,7 +644,7 @@
   <dimension ref="A1:Y19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -730,7 +730,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="21"/>
-      <c r="C2" s="33"/>
+      <c r="C2" s="35"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
@@ -762,8 +762,8 @@
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="9"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="20"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="11"/>
@@ -811,7 +811,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="21"/>
-      <c r="C5" s="20"/>
+      <c r="C5" s="21"/>
       <c r="D5" s="11"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -838,7 +838,7 @@
       <c r="B6" s="32">
         <v>4</v>
       </c>
-      <c r="C6" s="35"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
@@ -859,7 +859,7 @@
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="20"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="9"/>
       <c r="D7" s="10"/>
       <c r="E7" s="9"/>
@@ -882,7 +882,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="30"/>
-      <c r="C8" s="34"/>
+      <c r="C8" s="33"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>

</xml_diff>

<commit_message>
PiI 5lab and fix results
</commit_message>
<xml_diff>
--- a/3-2 labs.xlsx
+++ b/3-2 labs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSTU\3\3-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E389390D-87EA-40F6-A4B9-DEAB6AAE8180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4A2FA0-D209-471C-BB64-FF31E1E9498F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3CBCB977-0A19-4CE0-8F0F-0CE5EBE89482}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>Предметы</t>
   </si>
@@ -36,9 +36,6 @@
     <t>РИС</t>
   </si>
   <si>
-    <t>ПвI</t>
-  </si>
-  <si>
     <t>ПМАиПЛ</t>
   </si>
   <si>
@@ -48,32 +45,35 @@
     <t>ОИАД</t>
   </si>
   <si>
-    <t>ЗИиНИС</t>
-  </si>
-  <si>
     <t>АИСиWП</t>
   </si>
   <si>
     <t>СП</t>
   </si>
   <si>
-    <t>ЗИиНИС курсач</t>
-  </si>
-  <si>
-    <t>БД курсач</t>
-  </si>
-  <si>
     <t>Зачет</t>
   </si>
   <si>
-    <t>30%(Табл. Word)</t>
+    <t>Защита</t>
+  </si>
+  <si>
+    <t>2. ЗИиНИС курсач</t>
+  </si>
+  <si>
+    <t>3. БД курсач</t>
+  </si>
+  <si>
+    <t>1. ЗИиНИС</t>
+  </si>
+  <si>
+    <t>4. ОПиПЧ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +132,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -171,7 +179,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -233,11 +241,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -259,25 +278,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -287,28 +291,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -318,22 +303,62 @@
     <xf numFmtId="9" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -653,12 +678,12 @@
   <dimension ref="A1:Y19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
     <col min="4" max="4" width="9.88671875" customWidth="1"/>
     <col min="12" max="12" width="9" customWidth="1"/>
   </cols>
@@ -715,198 +740,164 @@
       <c r="Q1" s="1">
         <v>16</v>
       </c>
-      <c r="R1" s="6">
-        <v>17</v>
-      </c>
-      <c r="S1" s="6">
-        <v>18</v>
-      </c>
-      <c r="T1" s="6">
-        <v>19</v>
-      </c>
-      <c r="U1" s="6">
-        <v>20</v>
-      </c>
-      <c r="V1" s="6">
-        <v>21</v>
-      </c>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="25" t="s">
         <v>1</v>
       </c>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="28"/>
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
-      <c r="Y2" s="19"/>
+      <c r="Y2" s="14"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="28" t="s">
+      <c r="A3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="C3" s="21">
         <v>1</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>9</v>
       </c>
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="27" t="s">
+      <c r="A4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="39">
+        <v>0.3</v>
+      </c>
+      <c r="C4" s="39">
         <v>1</v>
       </c>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
+      <c r="D4" s="40" t="s">
+        <v>9</v>
+      </c>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="L5" s="21"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
+      <c r="A5" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="22" t="s">
+        <v>8</v>
+      </c>
       <c r="S5" s="8"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="30">
-        <v>4</v>
-      </c>
-      <c r="C6" s="30">
-        <v>8</v>
-      </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="35" t="s">
+        <v>1</v>
+      </c>
       <c r="R6" s="8"/>
       <c r="S6" s="8"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
       <c r="S7" s="8"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8" s="8"/>
+      <c r="A8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="18">
+        <v>4</v>
+      </c>
+      <c r="C8" s="18">
+        <v>8</v>
+      </c>
+      <c r="D8" s="18">
+        <v>8</v>
+      </c>
+      <c r="E8" s="18">
+        <v>6</v>
+      </c>
+      <c r="F8" s="20"/>
+      <c r="G8" s="18">
+        <v>8</v>
+      </c>
+      <c r="H8" s="20"/>
+      <c r="I8" s="37" t="s">
+        <v>8</v>
+      </c>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
       <c r="O8" s="8"/>
       <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
@@ -915,46 +906,70 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="9"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="10"/>
       <c r="E9" s="9"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="29" t="s">
+        <v>1</v>
+      </c>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="34">
-        <v>0.3</v>
-      </c>
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="41"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="35" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="A11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
     </row>
     <row r="18" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M18" s="3"/>

</xml_diff>

<commit_message>
AISaWP 10-11 and DIS 7
</commit_message>
<xml_diff>
--- a/3-2 labs.xlsx
+++ b/3-2 labs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSTU\3\3-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC5C6B9-785E-4834-89FB-AADE83EEA733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFC0F9A-2674-4F41-A5FF-726285CCD9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3CBCB977-0A19-4CE0-8F0F-0CE5EBE89482}"/>
   </bookViews>
@@ -294,9 +294,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -365,6 +362,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -684,7 +684,7 @@
   <dimension ref="A1:Y19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -765,23 +765,23 @@
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
-      <c r="H2" s="28"/>
+      <c r="H2" s="27"/>
       <c r="I2" s="14"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="20" t="s">
+      <c r="J2" s="28"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="R2" s="4"/>
-      <c r="S2" s="24"/>
+      <c r="S2" s="23"/>
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
-      <c r="V2" s="25"/>
+      <c r="V2" s="24"/>
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
       <c r="Y2" s="13"/>
@@ -799,10 +799,10 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
       <c r="J3" s="14"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="23" t="s">
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="22" t="s">
         <v>1</v>
       </c>
       <c r="R3" s="8"/>
@@ -812,55 +812,55 @@
       <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="16">
         <v>4</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="16">
         <v>8</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="16">
         <v>8</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="16">
         <v>6</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="16">
         <v>5</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="16">
         <v>8</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="16">
         <v>7</v>
       </c>
-      <c r="I4" s="38" t="s">
+      <c r="I4" s="37" t="s">
         <v>6</v>
       </c>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="20"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="19"/>
       <c r="S5" s="8"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="18">
         <v>0.3</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="18">
         <v>1</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="19" t="s">
         <v>7</v>
       </c>
       <c r="R6" s="8"/>
@@ -870,13 +870,13 @@
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="34">
+      <c r="B7" s="33">
         <v>0.3</v>
       </c>
-      <c r="C7" s="34">
+      <c r="C7" s="33">
         <v>1</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="34" t="s">
         <v>7</v>
       </c>
       <c r="R7" s="8"/>
@@ -888,7 +888,7 @@
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
-      <c r="D8" s="27"/>
+      <c r="D8" s="26"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
@@ -898,7 +898,7 @@
       <c r="K8" s="9"/>
       <c r="L8" s="11"/>
       <c r="M8" s="9"/>
-      <c r="N8" s="26" t="s">
+      <c r="N8" s="25" t="s">
         <v>1</v>
       </c>
       <c r="R8" s="8"/>
@@ -908,14 +908,14 @@
       <c r="A9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="31"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="30"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="37" t="s">
+      <c r="I9" s="36" t="s">
         <v>6</v>
       </c>
       <c r="R9" s="8"/>
@@ -926,13 +926,13 @@
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
-      <c r="D10" s="41" t="s">
+      <c r="D10" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="32"/>
+      <c r="E10" s="31"/>
       <c r="F10" s="10"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="26" t="s">
+      <c r="H10" s="25" t="s">
         <v>1</v>
       </c>
       <c r="J10" s="8"/>
@@ -946,11 +946,11 @@
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="40" t="s">
+      <c r="F11" s="38"/>
+      <c r="G11" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="36"/>
+      <c r="H11" s="35"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
@@ -962,11 +962,11 @@
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="15" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="41" t="s">
         <v>1</v>
       </c>
       <c r="H12" s="8"/>

</xml_diff>

<commit_message>
AISaWP FULL and PiI 7
</commit_message>
<xml_diff>
--- a/3-2 labs.xlsx
+++ b/3-2 labs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSTU\3\3-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52139204-EED8-4BE1-9437-62B1598601C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFD9062-9F66-4CC8-ACD5-D34B68A5F3F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3CBCB977-0A19-4CE0-8F0F-0CE5EBE89482}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Предметы</t>
   </si>
@@ -33,12 +33,6 @@
     <t>Конец</t>
   </si>
   <si>
-    <t>АПвП</t>
-  </si>
-  <si>
-    <t>АИСиWП</t>
-  </si>
-  <si>
     <t>СП</t>
   </si>
   <si>
@@ -73,13 +67,19 @@
   </si>
   <si>
     <t>7. РИС</t>
+  </si>
+  <si>
+    <t>8. АПвП</t>
+  </si>
+  <si>
+    <t>9. АИСиWП</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,14 +115,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -147,7 +139,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,6 +170,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -256,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -278,48 +276,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -340,9 +335,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -352,10 +344,8 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -675,7 +665,7 @@
   <dimension ref="A1:Y19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12:G12"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -737,209 +727,200 @@
       <c r="Q1" s="1">
         <v>16</v>
       </c>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="18" t="s">
         <v>1</v>
       </c>
       <c r="R2" s="4"/>
-      <c r="S2" s="23"/>
+      <c r="S2" s="22"/>
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
-      <c r="V2" s="24"/>
+      <c r="V2" s="23"/>
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
-      <c r="Y2" s="13"/>
+      <c r="Y2" s="12"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="21" t="s">
         <v>1</v>
       </c>
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="16">
-        <v>4</v>
-      </c>
-      <c r="C4" s="16">
-        <v>8</v>
-      </c>
-      <c r="D4" s="16">
-        <v>8</v>
-      </c>
-      <c r="E4" s="16">
-        <v>6</v>
-      </c>
-      <c r="F4" s="16">
-        <v>5</v>
-      </c>
-      <c r="G4" s="16">
-        <v>8</v>
-      </c>
-      <c r="H4" s="16">
-        <v>7</v>
-      </c>
-      <c r="I4" s="37" t="s">
-        <v>5</v>
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="27" t="s">
+        <v>1</v>
       </c>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="19"/>
+      <c r="B5" s="15">
+        <v>4</v>
+      </c>
+      <c r="C5" s="15">
+        <v>8</v>
+      </c>
+      <c r="D5" s="15">
+        <v>8</v>
+      </c>
+      <c r="E5" s="15">
+        <v>6</v>
+      </c>
+      <c r="F5" s="15">
+        <v>5</v>
+      </c>
+      <c r="G5" s="15">
+        <v>8</v>
+      </c>
+      <c r="H5" s="15">
+        <v>7</v>
+      </c>
+      <c r="I5" s="35"/>
       <c r="S5" s="8"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="37" t="s">
-        <v>1</v>
-      </c>
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="38"/>
       <c r="R6" s="8"/>
       <c r="S6" s="8"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="18">
-        <v>0.3</v>
-      </c>
-      <c r="C7" s="18">
-        <v>1</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>6</v>
-      </c>
+      <c r="A7" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="18"/>
       <c r="R7" s="8"/>
       <c r="S7" s="8"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="33">
-        <v>0.3</v>
-      </c>
-      <c r="C8" s="33">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="35" t="s">
         <v>1</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>6</v>
       </c>
       <c r="R8" s="8"/>
       <c r="S8" s="8"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="25" t="s">
+      <c r="A9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="17">
+        <v>0.3</v>
+      </c>
+      <c r="C9" s="17">
         <v>1</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>4</v>
       </c>
       <c r="R9" s="8"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="36" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="B10" s="32">
+        <v>0.3</v>
+      </c>
+      <c r="C10" s="32">
+        <v>1</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="31"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
+      <c r="A11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="34" t="s">
+        <v>3</v>
+      </c>
       <c r="O11" s="8"/>
       <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
@@ -948,37 +929,36 @@
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="H12" s="35"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="30"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="24" t="s">
+        <v>1</v>
+      </c>
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
       <c r="Q12" s="8"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
       <c r="O13" s="8"/>
       <c r="P13" s="8"/>
       <c r="Q13" s="8"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
     </row>
     <row r="18" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M18" s="3"/>

</xml_diff>

<commit_message>
SP Upload + exams
</commit_message>
<xml_diff>
--- a/3-2 labs.xlsx
+++ b/3-2 labs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSTU\3\3-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDC33DB-6431-4667-8FCE-33012960C6B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55738C37-61D7-433B-BF14-2025BAE1866F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3CBCB977-0A19-4CE0-8F0F-0CE5EBE89482}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Предметы</t>
   </si>
@@ -36,9 +36,6 @@
     <t>СП</t>
   </si>
   <si>
-    <t>Зачет</t>
-  </si>
-  <si>
     <t>Защита</t>
   </si>
   <si>
@@ -54,9 +51,6 @@
     <t>4. ОПиПЧ</t>
   </si>
   <si>
-    <t>ПвI</t>
-  </si>
-  <si>
     <t>5. ПМАиПЛ</t>
   </si>
   <si>
@@ -73,6 +67,9 @@
   </si>
   <si>
     <t>Теория</t>
+  </si>
+  <si>
+    <t>10. ПвI</t>
   </si>
 </sst>
 </file>
@@ -160,13 +157,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -248,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -267,9 +264,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -331,10 +325,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -654,7 +648,7 @@
   <dimension ref="A1:Y19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -716,63 +710,63 @@
       <c r="Q1" s="1">
         <v>16</v>
       </c>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="17" t="s">
         <v>1</v>
       </c>
       <c r="R2" s="4"/>
-      <c r="S2" s="22"/>
+      <c r="S2" s="21"/>
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
-      <c r="V2" s="23"/>
+      <c r="V2" s="22"/>
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
-      <c r="Y2" s="12"/>
+      <c r="Y2" s="11"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="20" t="s">
         <v>1</v>
       </c>
       <c r="R3" s="8"/>
@@ -780,134 +774,128 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="27" t="s">
-        <v>1</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="26"/>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="15">
+        <v>8</v>
+      </c>
+      <c r="B5" s="14">
         <v>4</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <v>8</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <v>8</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>6</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="14">
         <v>5</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="14">
         <v>8</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="14">
         <v>7</v>
       </c>
-      <c r="I5" s="32"/>
+      <c r="I5" s="31"/>
       <c r="S5" s="8"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
+      <c r="A6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
       <c r="F6" s="27"/>
-      <c r="G6" s="33"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="17"/>
       <c r="R6" s="8"/>
       <c r="S6" s="8"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="18"/>
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="32"/>
       <c r="R7" s="8"/>
       <c r="S7" s="8"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="32" t="s">
-        <v>1</v>
-      </c>
+      <c r="A8" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="17"/>
       <c r="R8" s="8"/>
       <c r="S8" s="8"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="17">
-        <v>0.3</v>
-      </c>
-      <c r="C9" s="17">
-        <v>1</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>4</v>
-      </c>
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="31"/>
       <c r="R9" s="8"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="30">
+        <v>4</v>
+      </c>
+      <c r="B10" s="16">
         <v>0.3</v>
       </c>
-      <c r="C10" s="30">
+      <c r="C10" s="16">
         <v>1</v>
       </c>
-      <c r="D10" s="31" t="s">
-        <v>4</v>
+      <c r="D10" s="17" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="29">
+        <v>0.3</v>
+      </c>
+      <c r="C11" s="29">
+        <v>1</v>
+      </c>
+      <c r="D11" s="30" t="s">
         <v>3</v>
       </c>
       <c r="O11" s="8"/>
@@ -918,15 +906,15 @@
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="10"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="34"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="23" t="s">
         <v>1</v>
       </c>
       <c r="O12" s="8"/>

</xml_diff>

<commit_message>
Full SP and Practice
</commit_message>
<xml_diff>
--- a/3-2 labs.xlsx
+++ b/3-2 labs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSTU\3\3-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55FE8AF-86E9-4C3A-9BD5-295DFCCC2887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2416CA5F-8B5F-4F04-8C2A-6D93612549E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3CBCB977-0A19-4CE0-8F0F-0CE5EBE89482}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Предметы</t>
   </si>
@@ -33,12 +33,6 @@
     <t>Конец</t>
   </si>
   <si>
-    <t>СП</t>
-  </si>
-  <si>
-    <t>Защита</t>
-  </si>
-  <si>
     <t>2. ЗИиНИС курсач</t>
   </si>
   <si>
@@ -66,10 +60,10 @@
     <t>9. АИСиWП</t>
   </si>
   <si>
-    <t>Теория</t>
-  </si>
-  <si>
     <t>10. ПвI</t>
+  </si>
+  <si>
+    <t>11. СП</t>
   </si>
 </sst>
 </file>
@@ -136,7 +130,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,26 +143,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -211,19 +187,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -245,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -283,11 +246,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -306,29 +269,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -648,7 +593,7 @@
   <dimension ref="A1:Y19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -721,7 +666,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -738,9 +683,7 @@
       <c r="N2" s="25"/>
       <c r="O2" s="25"/>
       <c r="P2" s="25"/>
-      <c r="Q2" s="16" t="s">
-        <v>1</v>
-      </c>
+      <c r="Q2" s="16"/>
       <c r="R2" s="4"/>
       <c r="S2" s="20"/>
       <c r="T2" s="3"/>
@@ -752,7 +695,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -766,15 +709,13 @@
       <c r="K3" s="17"/>
       <c r="L3" s="17"/>
       <c r="M3" s="18"/>
-      <c r="N3" s="19" t="s">
-        <v>1</v>
-      </c>
+      <c r="N3" s="19"/>
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -794,35 +735,21 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="13">
-        <v>4</v>
-      </c>
-      <c r="C5" s="13">
-        <v>8</v>
-      </c>
-      <c r="D5" s="13">
-        <v>8</v>
-      </c>
-      <c r="E5" s="13">
         <v>6</v>
       </c>
-      <c r="F5" s="13">
-        <v>5</v>
-      </c>
-      <c r="G5" s="13">
-        <v>8</v>
-      </c>
-      <c r="H5" s="13">
-        <v>7</v>
-      </c>
-      <c r="I5" s="29"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="27"/>
       <c r="S5" s="8"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
@@ -837,86 +764,81 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="D7" s="13"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="30"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="24" t="s">
+        <v>1</v>
+      </c>
       <c r="R7" s="8"/>
       <c r="S7" s="8"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A8" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="16"/>
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="28"/>
       <c r="R8" s="8"/>
       <c r="S8" s="8"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="29"/>
+      <c r="A9" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="16"/>
+      <c r="H9" s="8"/>
       <c r="R9" s="8"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="C10" s="15">
-        <v>1</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>3</v>
-      </c>
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="27"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="27">
+        <v>2</v>
+      </c>
+      <c r="B11" s="15">
         <v>0.3</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="15">
         <v>1</v>
       </c>
-      <c r="D11" s="28" t="s">
-        <v>3</v>
-      </c>
+      <c r="D11" s="16"/>
       <c r="O11" s="8"/>
       <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="32"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="34" t="s">
+      <c r="A12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="C12" s="15">
         <v>1</v>
       </c>
+      <c r="D12" s="16"/>
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
       <c r="Q12" s="8"/>
@@ -929,7 +851,6 @@
       <c r="Q13" s="8"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="H14" s="8"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>

</xml_diff>